<commit_message>
styling for xls report
</commit_message>
<xml_diff>
--- a/backend/reports/GIRLS_Absent_Students_2024-11-22.xlsx
+++ b/backend/reports/GIRLS_Absent_Students_2024-11-22.xlsx
@@ -86,7 +86,8 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,13 +117,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,7 +465,7 @@
   <dimension ref="A1:E8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" ht="25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,7 +474,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" ht="25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -483,7 +483,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" ht="25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -492,7 +492,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" ht="25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -509,71 +509,71 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+    <row r="5" ht="25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="6" ht="25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+    <row r="7" ht="25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+    <row r="8" ht="25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>